<commit_message>
inserção de dados de temperatura de plantas
</commit_message>
<xml_diff>
--- a/Levantamento de dados/DadosCF.xlsx
+++ b/Levantamento de dados/DadosCF.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael Bachega\Desktop\Plant.ai\Levantamento de dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Nova pasta\Plant.ai\Levantamento de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5057097B-8753-4039-9108-F103E50EEC07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0823508B-B4BD-43C4-811C-6268FD8A6D2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Preços" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Tipos de plantas</t>
   </si>
@@ -88,17 +88,89 @@
   </si>
   <si>
     <t>G1.</t>
+  </si>
+  <si>
+    <t>Planta</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>IdPlanta</t>
+  </si>
+  <si>
+    <t>Tomate</t>
+  </si>
+  <si>
+    <t>Fruta</t>
+  </si>
+  <si>
+    <t>Temperatura Miníma (ºC)</t>
+  </si>
+  <si>
+    <t>Temperatura Maxíma(ºC)</t>
+  </si>
+  <si>
+    <t>Temp. Min. Ideal (ºC)</t>
+  </si>
+  <si>
+    <t>Temp. Max. Ideal (ºC)</t>
+  </si>
+  <si>
+    <t>Batata</t>
+  </si>
+  <si>
+    <t>legume</t>
+  </si>
+  <si>
+    <t>Cenoura</t>
+  </si>
+  <si>
+    <t>Legume</t>
+  </si>
+  <si>
+    <t>Beterraba</t>
+  </si>
+  <si>
+    <t>Abobrinha</t>
+  </si>
+  <si>
+    <t>Alface</t>
+  </si>
+  <si>
+    <t>Verdura</t>
+  </si>
+  <si>
+    <t>Acelga</t>
+  </si>
+  <si>
+    <t>Brocólis</t>
+  </si>
+  <si>
+    <t>Chuchu</t>
+  </si>
+  <si>
+    <t>Couve-flor</t>
+  </si>
+  <si>
+    <t>Orquídeas</t>
+  </si>
+  <si>
+    <t>Flor</t>
+  </si>
+  <si>
+    <t>Tempo médio de germinação (Dias) / (vezes ao ano)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +184,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Rounded MT Bold"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -140,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -247,20 +325,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -277,10 +370,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -591,10 +689,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D8F8C58-4AC5-4978-AA9D-52FFD3D51BDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -764,4 +862,347 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>34</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>24</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>24</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>19</v>
+      </c>
+      <c r="H8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>19</v>
+      </c>
+      <c r="H9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>21</v>
+      </c>
+      <c r="G10">
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>27</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>15</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>35</v>
+      </c>
+      <c r="F13">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <v>28</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
inserção de novos dados
</commit_message>
<xml_diff>
--- a/Levantamento de dados/DadosCF.xlsx
+++ b/Levantamento de dados/DadosCF.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Nova pasta\Plant.ai\Levantamento de dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\Plant.ai\Levantamento de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Tipos de plantas</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Tempo médio de germinação (Dias) / (vezes ao ano)</t>
+  </si>
+  <si>
+    <t>Salsinha</t>
+  </si>
+  <si>
+    <t>Pimenta-vermelha</t>
   </si>
 </sst>
 </file>
@@ -693,7 +699,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,16 +872,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
@@ -1131,7 +1137,7 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>13</v>
@@ -1199,6 +1205,66 @@
       </c>
       <c r="H13">
         <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>22</v>
+      </c>
+      <c r="H14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>30</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>35</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>